<commit_message>
REPORTGEN-885: fix bad configuration in templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Security Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Security Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D649D3C-B9D7-43D7-9F2F-A6F08364F28C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EAD447-F5D7-4386-BD78-00125E7DC1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Rules</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CISQ-Security,MORE=true,HEADER=NO</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Security,DESC=true,HEADER=NO</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Security,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CISQ-Security,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -813,26 +813,26 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="75.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="75.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
@@ -884,10 +884,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
@@ -898,13 +898,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
@@ -912,7 +912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>18</v>
       </c>
@@ -920,12 +920,12 @@
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="34.200000000000003" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
@@ -939,9 +939,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -965,18 +965,18 @@
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -990,18 +990,18 @@
         <v>22</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1024,47 +1024,47 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>